<commit_message>
Implemetación formulario de edición: Ahora permite subir imágene y marcar si es confiable o no el registro
</commit_message>
<xml_diff>
--- a/public/file/ReportDatPaq.xlsx
+++ b/public/file/ReportDatPaq.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jedat\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\reportdatpaq\public\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B0EFD2-968B-417C-8514-2F61B6AAEBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD9EA57-6B05-4519-85EF-2B0B2047F518}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -547,7 +547,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -903,96 +903,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD14"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="11.42578125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>